<commit_message>
finalize the draft version
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-np-core-immunization.xlsx
+++ b/output/StructureDefinition-np-core-immunization.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="424">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-20T08:30:34+05:45</t>
+    <t>2025-08-29T13:54:08+05:45</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -472,10 +472,14 @@
     <t>Immunization.modifierExtension</t>
   </si>
   <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>An Extension</t>
+    <t>Extensions that cannot be ignored</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource and that modifies the understanding of the element that contains it and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and managable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
+  </si>
+  <si>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R5/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -714,7 +718,7 @@
     <t>Immunization.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://fhir.hmis.gov.np/StructureDefinition/np-core-encounter)
+    <t xml:space="preserve">Reference(Encounter)
 </t>
   </si>
   <si>
@@ -991,9 +995,6 @@
   <si>
     <t>May be used to represent additional information that is not part of the basic definition of the element and that modifies the understanding of the element in which it is contained and/or the understanding of the containing element's descendants. Usually modifier elements provide negation or qualification. To make the use of extensions safe and managable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
-  </si>
-  <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R5/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>BackboneElement.modifierExtension</t>
@@ -2179,7 +2180,7 @@
         <v>81</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>80</v>
@@ -2530,7 +2531,7 @@
         <v>81</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H8" t="s" s="2">
         <v>80</v>
@@ -2757,14 +2758,14 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
         <v>81</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>80</v>
@@ -2784,8 +2785,12 @@
       <c r="M10" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="N10" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="O10" t="s" s="2">
+        <v>149</v>
+      </c>
       <c r="P10" t="s" s="2">
         <v>80</v>
       </c>
@@ -2833,7 +2838,7 @@
         <v>80</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>81</v>
@@ -2857,7 +2862,7 @@
         <v>80</v>
       </c>
       <c r="AN10" t="s" s="2">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="AO10" t="s" s="2">
         <v>80</v>
@@ -2865,10 +2870,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2891,13 +2896,13 @@
         <v>80</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2948,7 +2953,7 @@
         <v>80</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>81</v>
@@ -2963,27 +2968,27 @@
         <v>104</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AM11" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AO11" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -3006,16 +3011,16 @@
         <v>93</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" t="s" s="2">
@@ -3065,7 +3070,7 @@
         <v>80</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>81</v>
@@ -3080,7 +3085,7 @@
         <v>104</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>80</v>
@@ -3097,10 +3102,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -3126,13 +3131,13 @@
         <v>112</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
@@ -3143,7 +3148,7 @@
         <v>80</v>
       </c>
       <c r="S13" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="T13" t="s" s="2">
         <v>80</v>
@@ -3162,7 +3167,7 @@
       </c>
       <c r="Y13" s="2"/>
       <c r="Z13" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AA13" t="s" s="2">
         <v>80</v>
@@ -3180,7 +3185,7 @@
         <v>80</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>92</v>
@@ -3195,16 +3200,16 @@
         <v>104</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AM13" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>80</v>
@@ -3212,10 +3217,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3238,16 +3243,16 @@
         <v>80</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
@@ -3273,11 +3278,11 @@
         <v>80</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y14" s="2"/>
       <c r="Z14" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>80</v>
@@ -3295,7 +3300,7 @@
         <v>80</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>81</v>
@@ -3310,7 +3315,7 @@
         <v>104</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>80</v>
@@ -3319,7 +3324,7 @@
         <v>80</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>80</v>
@@ -3327,10 +3332,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3353,16 +3358,16 @@
         <v>93</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
@@ -3392,7 +3397,7 @@
       </c>
       <c r="Y15" s="2"/>
       <c r="Z15" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>80</v>
@@ -3410,7 +3415,7 @@
         <v>80</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>92</v>
@@ -3425,27 +3430,27 @@
         <v>104</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AO15" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3468,13 +3473,13 @@
         <v>80</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -3525,7 +3530,7 @@
         <v>80</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>81</v>
@@ -3540,27 +3545,27 @@
         <v>104</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3583,13 +3588,13 @@
         <v>80</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -3640,7 +3645,7 @@
         <v>80</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>81</v>
@@ -3661,21 +3666,21 @@
         <v>80</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3698,13 +3703,13 @@
         <v>80</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3755,7 +3760,7 @@
         <v>80</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>81</v>
@@ -3776,21 +3781,21 @@
         <v>80</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3813,13 +3818,13 @@
         <v>80</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -3870,7 +3875,7 @@
         <v>80</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>81</v>
@@ -3891,10 +3896,10 @@
         <v>80</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>80</v>
@@ -3902,10 +3907,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3928,13 +3933,13 @@
         <v>93</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -3985,7 +3990,7 @@
         <v>80</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>92</v>
@@ -4000,16 +4005,16 @@
         <v>104</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>80</v>
@@ -4017,10 +4022,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4043,13 +4048,13 @@
         <v>80</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -4100,7 +4105,7 @@
         <v>80</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>81</v>
@@ -4115,16 +4120,16 @@
         <v>104</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>80</v>
@@ -4132,10 +4137,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4158,13 +4163,13 @@
         <v>80</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -4215,7 +4220,7 @@
         <v>80</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>81</v>
@@ -4233,7 +4238,7 @@
         <v>80</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>80</v>
@@ -4247,10 +4252,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4273,16 +4278,16 @@
         <v>93</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -4320,17 +4325,17 @@
         <v>80</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>92</v>
@@ -4345,30 +4350,30 @@
         <v>104</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D24" t="s" s="2">
         <v>80</v>
@@ -4390,16 +4395,16 @@
         <v>93</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -4449,7 +4454,7 @@
         <v>80</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>92</v>
@@ -4464,27 +4469,27 @@
         <v>104</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4507,16 +4512,16 @@
         <v>93</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
@@ -4566,7 +4571,7 @@
         <v>80</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>81</v>
@@ -4581,16 +4586,16 @@
         <v>104</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>80</v>
@@ -4598,10 +4603,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4624,16 +4629,16 @@
         <v>80</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
@@ -4659,11 +4664,11 @@
         <v>80</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y26" s="2"/>
       <c r="Z26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>80</v>
@@ -4681,7 +4686,7 @@
         <v>80</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>81</v>
@@ -4696,16 +4701,16 @@
         <v>104</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>80</v>
@@ -4713,10 +4718,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4739,13 +4744,13 @@
         <v>80</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4796,7 +4801,7 @@
         <v>80</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>81</v>
@@ -4811,16 +4816,16 @@
         <v>104</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>80</v>
@@ -4828,10 +4833,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4854,13 +4859,13 @@
         <v>80</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -4887,11 +4892,11 @@
         <v>80</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y28" s="2"/>
       <c r="Z28" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>80</v>
@@ -4909,7 +4914,7 @@
         <v>80</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>81</v>
@@ -4930,21 +4935,21 @@
         <v>80</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4967,13 +4972,13 @@
         <v>80</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5000,11 +5005,11 @@
         <v>80</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y29" s="2"/>
       <c r="Z29" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AA29" t="s" s="2">
         <v>80</v>
@@ -5022,7 +5027,7 @@
         <v>80</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>81</v>
@@ -5043,21 +5048,21 @@
         <v>80</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5080,13 +5085,13 @@
         <v>80</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -5137,7 +5142,7 @@
         <v>80</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>81</v>
@@ -5158,10 +5163,10 @@
         <v>80</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>80</v>
@@ -5169,10 +5174,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5195,13 +5200,13 @@
         <v>93</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -5252,7 +5257,7 @@
         <v>80</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>81</v>
@@ -5267,16 +5272,16 @@
         <v>104</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>80</v>
@@ -5284,10 +5289,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5310,13 +5315,13 @@
         <v>80</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5367,7 +5372,7 @@
         <v>80</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>81</v>
@@ -5376,7 +5381,7 @@
         <v>92</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>80</v>
@@ -5391,7 +5396,7 @@
         <v>80</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>80</v>
@@ -5399,10 +5404,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5431,7 +5436,7 @@
         <v>141</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N33" t="s" s="2">
         <v>143</v>
@@ -5484,7 +5489,7 @@
         <v>80</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>81</v>
@@ -5508,7 +5513,7 @@
         <v>80</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO33" t="s" s="2">
         <v>80</v>
@@ -5516,14 +5521,14 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
@@ -5545,16 +5550,16 @@
         <v>140</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="N34" t="s" s="2">
         <v>143</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>314</v>
+        <v>149</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>80</v>
@@ -5661,7 +5666,7 @@
         <v>93</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L35" t="s" s="2">
         <v>317</v>
@@ -6039,7 +6044,7 @@
         <v>80</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y38" s="2"/>
       <c r="Z38" t="s" s="2">
@@ -6107,7 +6112,7 @@
         <v>81</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>80</v>
@@ -6119,7 +6124,7 @@
         <v>93</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L39" t="s" s="2">
         <v>346</v>
@@ -6238,7 +6243,7 @@
         <v>80</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L40" t="s" s="2">
         <v>352</v>
@@ -6271,7 +6276,7 @@
         <v>80</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y40" t="s" s="2">
         <v>354</v>
@@ -6353,7 +6358,7 @@
         <v>80</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L41" t="s" s="2">
         <v>357</v>
@@ -6434,7 +6439,7 @@
         <v>359</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>80</v>
@@ -6468,13 +6473,13 @@
         <v>80</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6525,7 +6530,7 @@
         <v>80</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>81</v>
@@ -6534,7 +6539,7 @@
         <v>92</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>80</v>
@@ -6549,7 +6554,7 @@
         <v>80</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>80</v>
@@ -6589,7 +6594,7 @@
         <v>141</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N43" t="s" s="2">
         <v>143</v>
@@ -6642,7 +6647,7 @@
         <v>80</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>81</v>
@@ -6666,7 +6671,7 @@
         <v>80</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>80</v>
@@ -6681,7 +6686,7 @@
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
@@ -6703,16 +6708,16 @@
         <v>140</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="N44" t="s" s="2">
         <v>143</v>
       </c>
       <c r="O44" t="s" s="2">
-        <v>314</v>
+        <v>149</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>80</v>
@@ -6819,7 +6824,7 @@
         <v>80</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L45" t="s" s="2">
         <v>364</v>
@@ -6852,7 +6857,7 @@
         <v>80</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y45" s="2"/>
       <c r="Z45" t="s" s="2">
@@ -6898,7 +6903,7 @@
         <v>80</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>80</v>
@@ -6932,7 +6937,7 @@
         <v>80</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L46" t="s" s="2">
         <v>368</v>
@@ -6965,7 +6970,7 @@
         <v>80</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y46" s="2"/>
       <c r="Z46" t="s" s="2">
@@ -7011,7 +7016,7 @@
         <v>80</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>80</v>
@@ -7045,7 +7050,7 @@
         <v>80</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L47" t="s" s="2">
         <v>372</v>
@@ -7078,7 +7083,7 @@
         <v>80</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y47" s="2"/>
       <c r="Z47" t="s" s="2">
@@ -7158,7 +7163,7 @@
         <v>80</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L48" t="s" s="2">
         <v>376</v>
@@ -7275,13 +7280,13 @@
         <v>80</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7332,7 +7337,7 @@
         <v>80</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>81</v>
@@ -7341,7 +7346,7 @@
         <v>92</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>80</v>
@@ -7356,7 +7361,7 @@
         <v>80</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>80</v>
@@ -7396,7 +7401,7 @@
         <v>141</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N50" t="s" s="2">
         <v>143</v>
@@ -7449,7 +7454,7 @@
         <v>80</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>81</v>
@@ -7473,7 +7478,7 @@
         <v>80</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>80</v>
@@ -7488,7 +7493,7 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
@@ -7510,16 +7515,16 @@
         <v>140</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="N51" t="s" s="2">
         <v>143</v>
       </c>
       <c r="O51" t="s" s="2">
-        <v>314</v>
+        <v>149</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>80</v>
@@ -7626,7 +7631,7 @@
         <v>80</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L52" t="s" s="2">
         <v>385</v>
@@ -7707,7 +7712,7 @@
         <v>387</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>80</v>
@@ -7856,7 +7861,7 @@
         <v>80</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="L54" t="s" s="2">
         <v>395</v>
@@ -7971,7 +7976,7 @@
         <v>80</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L55" t="s" s="2">
         <v>400</v>
@@ -8086,13 +8091,13 @@
         <v>80</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8143,7 +8148,7 @@
         <v>80</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>81</v>
@@ -8152,7 +8157,7 @@
         <v>92</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>80</v>
@@ -8167,7 +8172,7 @@
         <v>80</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>80</v>
@@ -8207,7 +8212,7 @@
         <v>141</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N57" t="s" s="2">
         <v>143</v>
@@ -8260,7 +8265,7 @@
         <v>80</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>81</v>
@@ -8284,7 +8289,7 @@
         <v>80</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AO57" t="s" s="2">
         <v>80</v>
@@ -8299,7 +8304,7 @@
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
@@ -8321,16 +8326,16 @@
         <v>140</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="N58" t="s" s="2">
         <v>143</v>
       </c>
       <c r="O58" t="s" s="2">
-        <v>314</v>
+        <v>149</v>
       </c>
       <c r="P58" t="s" s="2">
         <v>80</v>
@@ -8437,7 +8442,7 @@
         <v>80</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L59" t="s" s="2">
         <v>406</v>
@@ -8667,7 +8672,7 @@
         <v>80</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L61" t="s" s="2">
         <v>413</v>
@@ -8700,7 +8705,7 @@
         <v>80</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Y61" s="2"/>
       <c r="Z61" t="s" s="2">
@@ -8780,7 +8785,7 @@
         <v>80</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L62" t="s" s="2">
         <v>417</v>
@@ -8897,7 +8902,7 @@
         <v>80</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L63" t="s" s="2">
         <v>421</v>

</xml_diff>